<commit_message>
Added bubbleDiffusivity and BubbleCoalesence models
</commit_message>
<xml_diff>
--- a/tests/diffusivities/diffusivities.xlsx
+++ b/tests/diffusivities/diffusivities.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13980" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25720" windowHeight="15380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="bubble diff" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>BUCK</t>
   </si>
@@ -58,6 +59,30 @@
   </si>
   <si>
     <t>R or k</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>cm^5</t>
+  </si>
+  <si>
+    <t>um^5</t>
+  </si>
+  <si>
+    <t>Db</t>
+  </si>
+  <si>
+    <t>Qb</t>
+  </si>
+  <si>
+    <t>J/mol</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -109,8 +134,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -177,7 +204,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -208,6 +235,7 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -238,6 +266,7 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -570,7 +599,7 @@
   <dimension ref="C2:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1188,4 +1217,100 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:6">
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1">
+        <v>8.3144600000000004</v>
+      </c>
+    </row>
+    <row r="2" spans="4:6">
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6">
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.1900000000000001E-22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6">
+      <c r="E5" s="1">
+        <f>E4*100000000000000000000</f>
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6">
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>418400</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6">
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="4:6">
+      <c r="D10" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10:E11" si="0">$E$5/D10^3*EXP(-$E$6/$E$1/$E$2)</f>
+        <v>7.7197954721823517E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6">
+      <c r="D11" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2.2873468065725492E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>